<commit_message>
Files will download in sharepoint if not there in folder-In test sequence
</commit_message>
<xml_diff>
--- a/Input_Automation/DirectBuyItemPrice.xlsx
+++ b/Input_Automation/DirectBuyItemPrice.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rpadeveloper\Documents\UiPath\Fellowes_Validation\Input_Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EF343E9-C460-42FD-A206-60C2D7954F3A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE5028D5-CC3E-40A6-B71B-8A11E8C3AE6D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3217,7 +3217,7 @@
       <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>